<commit_message>
Complete quality_risks unit tests
Started key_metrics documentation and unit tests
</commit_message>
<xml_diff>
--- a/qualityplans/data/test_fileA.xlsx
+++ b/qualityplans/data/test_fileA.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\quality_improvement_plans\qualityplans\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BFFBC1-6589-4320-936D-DAB472DD716F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79D481E-E529-48B2-8016-93E5EC9879B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Not Quality Risk" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Key Metrics" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,6 +23,116 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Detail 1a</t>
+  </si>
+  <si>
+    <t>Detail 1b</t>
+  </si>
+  <si>
+    <t>Detail 1c</t>
+  </si>
+  <si>
+    <t>detail 1d</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0 (1 out)</t>
+  </si>
+  <si>
+    <t>Detail 2a</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Detail 2c</t>
+  </si>
+  <si>
+    <t>Detail 2d</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>dEtail 3c</t>
+  </si>
+  <si>
+    <t>Detail 3d</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>3$</t>
+  </si>
+  <si>
+    <t>Detail 4c</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36,12 +146,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -56,8 +172,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,12 +468,553 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D28DE3-A8FB-42A5-ADF9-DA8466743D80}">
-  <dimension ref="A1"/>
+  <dimension ref="B4:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
+        <v>220</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1">
+        <v>999</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1">
+        <v>666</v>
+      </c>
+      <c r="D27" s="1">
+        <v>7</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>